<commit_message>
Updates adding in functions, and user inputs
</commit_message>
<xml_diff>
--- a/test excel 1.xlsx
+++ b/test excel 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fau-my.sharepoint.com/personal/jmazurkiewic2022_fau_edu/Documents/Desktop/Jackson PDF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{2E9BD649-6FF2-4F8D-ACAA-DCB5A6E795C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56790A8D-D939-4A46-B871-F58C39CB820E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{2E9BD649-6FF2-4F8D-ACAA-DCB5A6E795C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A603C27-471D-42B6-8AF2-A96003F746AA}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{3FD5FADC-51CA-4112-9AE3-D5D20773432E}"/>
+    <workbookView xWindow="5085" yWindow="3735" windowWidth="21600" windowHeight="11295" xr2:uid="{3FD5FADC-51CA-4112-9AE3-D5D20773432E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>Job Address</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>L25</t>
+  </si>
+  <si>
+    <t>City_2</t>
   </si>
 </sst>
 </file>
@@ -1000,6 +1003,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1302,7 +1309,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,9 +1323,9 @@
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1350,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1</v>
+        <v>299</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>

</xml_diff>